<commit_message>
updated calibration files TTS, fopity, ETS
</commit_message>
<xml_diff>
--- a/InputData/elec/ETS/Electricity Technology Shareweights.xlsx
+++ b/InputData/elec/ETS/Electricity Technology Shareweights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\Canada\canada-eps\InputData\elec\ETS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\Canada\eps-canada\InputData\elec\ETS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DFC328-4E8F-4C6A-8053-CD7031FD0DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7176E81D-0A27-4142-A838-466CD2D84561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="19190" windowHeight="10070" activeTab="1" xr2:uid="{9B08635C-C98A-4192-B8F2-5981CE9EC6E6}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -583,14 +583,14 @@
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -598,77 +598,77 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -690,16 +690,16 @@
   <dimension ref="A1:AG17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B17"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -800,7 +800,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -902,7 +902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1004,109 +1004,108 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1208,7 +1207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1310,7 +1309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1412,7 +1411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1514,7 +1513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1616,7 +1615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1718,7 +1717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1820,7 +1819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1922,7 +1921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2024,7 +2023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2126,7 +2125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2228,7 +2227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -2330,106 +2329,106 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f t="shared" ref="B17" si="1">C17</f>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>